<commit_message>
Updated with the correction to time calculation.
</commit_message>
<xml_diff>
--- a/results/example1/CRN1/mcmc_summary.xlsx
+++ b/results/example1/CRN1/mcmc_summary.xlsx
@@ -495,7 +495,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -507,31 +507,31 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.1455148015807536</v>
+        <v>0.8501760114036275</v>
       </c>
       <c r="G2">
-        <v>0.3357338239189235</v>
+        <v>0.1291565590113278</v>
       </c>
       <c r="H2">
-        <v>3015127461370608</v>
+        <v>1.447907280199614E+18</v>
       </c>
       <c r="I2">
-        <v>-0.9113662918684257</v>
+        <v>-0.153584975624098</v>
       </c>
       <c r="J2">
-        <v>0.6691329589082087</v>
+        <v>-0.007732616684352993</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.6150591811991899</v>
       </c>
       <c r="L2">
-        <v>0.9990436777341662</v>
+        <v>1.121563450511849</v>
       </c>
       <c r="M2">
-        <v>0.839591201955121</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>2.378402778406679</v>
+        <v>0.1500191543621032</v>
       </c>
       <c r="O2">
         <v>4501</v>
@@ -551,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -563,31 +563,31 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1.557020442320044</v>
+        <v>0.0076414631584662</v>
       </c>
       <c r="G3">
-        <v>0.6896379328970955</v>
+        <v>0.08447820241948407</v>
       </c>
       <c r="H3">
-        <v>-7.239536400998072E+16</v>
+        <v>-1.061293294387152E+16</v>
       </c>
       <c r="I3">
-        <v>1.050479182344899</v>
+        <v>0.4516945429508499</v>
       </c>
       <c r="J3">
-        <v>0.64158785599562</v>
+        <v>-0.001589774102599029</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>2.166912129294289</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0.1564096867362808</v>
+        <v>0.9895578760275494</v>
       </c>
       <c r="N3">
-        <v>2.378402778406679</v>
+        <v>0.1500191543621032</v>
       </c>
       <c r="O3">
         <v>4501</v>
@@ -607,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -619,31 +619,31 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1.581879314047859</v>
+        <v>0.0003565913521299812</v>
       </c>
       <c r="G4">
-        <v>0.3651549812518561</v>
+        <v>0.01223163318571148</v>
       </c>
       <c r="H4">
-        <v>-3.071318473150698E+17</v>
+        <v>4.747236984261031E+16</v>
       </c>
       <c r="I4">
-        <v>0.7729531269459844</v>
+        <v>0.8722687363902777</v>
       </c>
       <c r="J4">
-        <v>0.6466260378834815</v>
+        <v>-0.0008500983906317937</v>
       </c>
       <c r="K4">
-        <v>0.6464088693922734</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>2.003529329418632</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.9991113085980893</v>
       </c>
       <c r="N4">
-        <v>2.378402778406679</v>
+        <v>0.1500191543621032</v>
       </c>
       <c r="O4">
         <v>4501</v>
@@ -663,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -675,31 +675,31 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.6628767241250745</v>
+        <v>0.9249944634425169</v>
       </c>
       <c r="G5">
-        <v>0.4127832633727558</v>
+        <v>0.1423367181911414</v>
       </c>
       <c r="H5">
-        <v>-1041874070867321</v>
+        <v>-1.842791083890418E+18</v>
       </c>
       <c r="I5">
-        <v>45.12844203473964</v>
+        <v>0.6437610425204559</v>
       </c>
       <c r="J5">
-        <v>0.9143429008968291</v>
+        <v>0.02764200895731305</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>0.6635441657487544</v>
       </c>
       <c r="L5">
-        <v>1.063974480480413</v>
+        <v>1.227159110107581</v>
       </c>
       <c r="M5">
-        <v>0.2721617418351477</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>1.520399211286647</v>
+        <v>0.07580466036226756</v>
       </c>
       <c r="O5">
         <v>4501</v>
@@ -719,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -731,31 +731,28 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1.392869898852909</v>
+        <v>4.653781548358664E-05</v>
       </c>
       <c r="G6">
-        <v>0.4428198504068688</v>
+        <v>0.003121851568369667</v>
       </c>
       <c r="H6">
-        <v>-3.959121469295821E+16</v>
-      </c>
-      <c r="I6">
-        <v>-34.55916976986162</v>
+        <v>2.289181470671327E+16</v>
       </c>
       <c r="J6">
-        <v>0.790198322065229</v>
+        <v>-0.0002222715939667628</v>
       </c>
       <c r="K6">
-        <v>0.8076846958261958</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>2.283306462567639</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>0.9997778271495223</v>
       </c>
       <c r="N6">
-        <v>1.520399211286647</v>
+        <v>0.07580466036226756</v>
       </c>
       <c r="O6">
         <v>4501</v>
@@ -775,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -787,31 +784,31 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.5078140441282669</v>
+        <v>0.01097788015030839</v>
       </c>
       <c r="G7">
-        <v>0.8222658079205279</v>
+        <v>0.1062416093779839</v>
       </c>
       <c r="H7">
-        <v>-1466341284924378</v>
+        <v>7340467833711607</v>
       </c>
       <c r="I7">
-        <v>-47.98334789053671</v>
+        <v>-1.892465721900112</v>
       </c>
       <c r="J7">
-        <v>0.928187625117697</v>
+        <v>-0.01067933391970033</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>2.054636965714882</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>0.7187291712952677</v>
+        <v>0.9862252832703844</v>
       </c>
       <c r="N7">
-        <v>1.520399211286647</v>
+        <v>0.07580466036226756</v>
       </c>
       <c r="O7">
         <v>4501</v>

</xml_diff>